<commit_message>
removed some log and reporter files
</commit_message>
<xml_diff>
--- a/Files/Data.xlsx
+++ b/Files/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -76,6 +76,21 @@
     </r>
   </si>
   <si>
+    <t>Simple Interest</t>
+  </si>
+  <si>
+    <t>Compounded Monthly</t>
+  </si>
+  <si>
+    <t>Compounded Quarterly</t>
+  </si>
+  <si>
+    <t>Compounded Half Yearly</t>
+  </si>
+  <si>
+    <t>Compounded Yearly</t>
+  </si>
+  <si>
     <t>Principle</t>
   </si>
   <si>
@@ -86,24 +101,6 @@
   </si>
   <si>
     <t>Frequency</t>
-  </si>
-  <si>
-    <t>Final Amount</t>
-  </si>
-  <si>
-    <t>Simple Interest</t>
-  </si>
-  <si>
-    <t>Compounded Monthly</t>
-  </si>
-  <si>
-    <t>Compounded Quarterly</t>
-  </si>
-  <si>
-    <t>Compounded Half Yearly</t>
-  </si>
-  <si>
-    <t>Compounded Yearly</t>
   </si>
   <si>
     <t xml:space="preserve">Maturity Value </t>
@@ -430,31 +427,31 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1765,7 +1762,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1775,101 +1772,78 @@
     <col min="2" max="2" width="20" style="25" customWidth="1"/>
     <col min="3" max="3" width="16.8516" style="25" customWidth="1"/>
     <col min="4" max="4" width="28.6719" style="25" customWidth="1"/>
-    <col min="5" max="5" width="19.3516" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="9.17188" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.17188" style="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="s" s="26">
+    <row r="1" ht="17.9" customHeight="1">
+      <c r="A1" s="26">
+        <v>5600</v>
+      </c>
+      <c r="B1" s="26">
+        <v>10</v>
+      </c>
+      <c r="C1" s="26">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="27">
         <v>12</v>
       </c>
-      <c r="B1" t="s" s="26">
+    </row>
+    <row r="2" ht="17.9" customHeight="1">
+      <c r="A2" s="26">
+        <v>6756</v>
+      </c>
+      <c r="B2" s="26">
+        <v>15</v>
+      </c>
+      <c r="C2" s="26">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="27">
         <v>13</v>
       </c>
-      <c r="C1" t="s" s="26">
+    </row>
+    <row r="3" ht="17.9" customHeight="1">
+      <c r="A3" s="26">
+        <v>8239</v>
+      </c>
+      <c r="B3" s="26">
+        <v>10</v>
+      </c>
+      <c r="C3" s="26">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s" s="27">
         <v>14</v>
       </c>
-      <c r="D1" t="s" s="26">
+    </row>
+    <row r="4" ht="17.9" customHeight="1">
+      <c r="A4" s="26">
+        <v>2534</v>
+      </c>
+      <c r="B4" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4" s="26">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s" s="27">
         <v>15</v>
       </c>
-      <c r="E1" t="s" s="26">
+    </row>
+    <row r="5" ht="17.9" customHeight="1">
+      <c r="A5" s="26">
+        <v>34231</v>
+      </c>
+      <c r="B5" s="26">
+        <v>8</v>
+      </c>
+      <c r="C5" s="26">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s" s="27">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="27">
-        <v>5600</v>
-      </c>
-      <c r="B2" s="27">
-        <v>10</v>
-      </c>
-      <c r="C2" s="27">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s" s="28">
-        <v>17</v>
-      </c>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="27">
-        <v>6756</v>
-      </c>
-      <c r="B3" s="27">
-        <v>15</v>
-      </c>
-      <c r="C3" s="27">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s" s="28">
-        <v>18</v>
-      </c>
-      <c r="E3" s="28"/>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="27">
-        <v>8239</v>
-      </c>
-      <c r="B4" s="27">
-        <v>10</v>
-      </c>
-      <c r="C4" s="27">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s" s="28">
-        <v>19</v>
-      </c>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="27">
-        <v>2534</v>
-      </c>
-      <c r="B5" s="27">
-        <v>6</v>
-      </c>
-      <c r="C5" s="27">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s" s="28">
-        <v>20</v>
-      </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="27">
-        <v>34231</v>
-      </c>
-      <c r="B6" s="27">
-        <v>8</v>
-      </c>
-      <c r="C6" s="27">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s" s="28">
-        <v>21</v>
-      </c>
-      <c r="E6" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1888,79 +1862,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.85156" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="30" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="28" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1979,65 +1953,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.3516" style="32" customWidth="1"/>
-    <col min="2" max="2" width="20" style="32" customWidth="1"/>
-    <col min="3" max="3" width="16.8516" style="32" customWidth="1"/>
-    <col min="4" max="4" width="18.1719" style="32" customWidth="1"/>
-    <col min="5" max="5" width="19.3516" style="32" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="32" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="32" customWidth="1"/>
+    <col min="1" max="1" width="11.3516" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20" style="30" customWidth="1"/>
+    <col min="3" max="3" width="16.8516" style="30" customWidth="1"/>
+    <col min="4" max="4" width="18.1719" style="30" customWidth="1"/>
+    <col min="5" max="5" width="19.3516" style="30" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="30" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" t="s" s="33">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s" s="33">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s" s="33">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s" s="33">
-        <v>15</v>
-      </c>
-      <c r="E1" t="s" s="34">
+      <c r="A1" t="s" s="31">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s" s="31">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s" s="33">
         <v>22</v>
       </c>
-      <c r="F1" t="s" s="26">
-        <v>23</v>
-      </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="35"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="35"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="35"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="35"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
@@ -2049,36 +2023,36 @@
       <c r="F6" s="36"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>